<commit_message>
Update with 4D box results
</commit_message>
<xml_diff>
--- a/4d_box_output.xlsx
+++ b/4d_box_output.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
@@ -464,7 +464,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16/6/2025 (Mon)</t>
+          <t>15/6/2025 (Sun)</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -483,8 +483,25 @@
       </c>
     </row>
     <row r="3" ht="60" customHeight="1">
-      <c r="B3" s="1" t="n"/>
-      <c r="C3" s="1" t="n"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>16/6/2025 (Mon)</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>2 9 3 2
+0 2 8 9
+8 5 2 5
+6 7 4 1</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>✅ Direct: 12/3547 (0.34%)
+✅ iBet: 12/195 (6.15%)</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="60" customHeight="1">
       <c r="B4" s="1" t="n"/>
@@ -496,6 +513,7 @@
     </row>
     <row r="6" ht="60" customHeight="1">
       <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
     </row>
     <row r="7" ht="60" customHeight="1">
       <c r="B7" s="1" t="n"/>
@@ -571,6 +589,9 @@
     </row>
     <row r="31">
       <c r="B31" s="1" t="n"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>